<commit_message>
Atualização lista requisitos helpdesk
</commit_message>
<xml_diff>
--- a/Pasta documentos requisitos/Aula 4 do parducci - Sobre requisitos funcionais do sistema.xlsx
+++ b/Pasta documentos requisitos/Aula 4 do parducci - Sobre requisitos funcionais do sistema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF316C0B-C73C-4DCC-9E37-231DD69FB348}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9465C3C6-AA6E-4BC3-B247-60BAC1A5903C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{A86947FA-8189-413F-B200-56D2539BABCB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Requisitos</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>Cada cliente só visualiza os seus pontos</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>funcional</t>
+  </si>
+  <si>
+    <t>não tem regra</t>
+  </si>
+  <si>
+    <t>negócio</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -152,11 +164,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -168,6 +191,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCCB550-A749-41C8-81FF-D631A0BE4524}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -606,6 +630,20 @@
       </c>
       <c r="D8" s="4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>